<commit_message>
a tuning record is added
</commit_message>
<xml_diff>
--- a/OttoProduct/xgb-param-tuning.xlsx
+++ b/OttoProduct/xgb-param-tuning.xlsx
@@ -878,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,6 +1042,38 @@
         <v>777</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.75</v>
+      </c>
+      <c r="C5">
+        <v>0.75</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>626</v>
+      </c>
+      <c r="F5">
+        <v>627</v>
+      </c>
+      <c r="G5">
+        <v>0.22</v>
+      </c>
+      <c r="H5">
+        <v>0.01</v>
+      </c>
+      <c r="I5">
+        <v>0.47</v>
+      </c>
+      <c r="J5">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>